<commit_message>
new lists of LI tickets/packs with prizes, also updated the packs used of games 363 and 444. File with list of codes errors to replicate in Hades.
</commit_message>
<xml_diff>
--- a/New Terminals/LI/LI_4patamares06092021.xlsx
+++ b/New Terminals/LI/LI_4patamares06092021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\105864\Documents\Millennium\New Terminals\LI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D91D14-0B9E-463A-ABDF-53ED132B2B86}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E7512D-0AFA-4428-8A32-C7A633C51828}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="194">
   <si>
     <t xml:space="preserve">Jogo </t>
   </si>
@@ -595,13 +595,28 @@
     <t>X</t>
   </si>
   <si>
-    <t>Coluna1</t>
-  </si>
-  <si>
     <t>HC</t>
   </si>
   <si>
-    <t>Coluna2</t>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Usado</t>
+  </si>
+  <si>
+    <t>Por Quem</t>
+  </si>
+  <si>
+    <t>Disponível (401)</t>
+  </si>
+  <si>
+    <t>Já cobrado (401431)</t>
+  </si>
+  <si>
+    <t>Já cobrado (400831)</t>
+  </si>
+  <si>
+    <t>AF</t>
   </si>
 </sst>
 </file>
@@ -613,7 +628,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00\ _€;\-#,##0.00\ _€"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -638,13 +653,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -863,9 +871,7 @@
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1244,16 +1250,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="B2:F59" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="B2:G59" totalsRowShown="0" headerRowDxfId="21">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:D59">
     <sortCondition ref="B2:B59"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Jogo " dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Nº série Transação Aposta" dataDxfId="19"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Valor prémio €" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{77371F62-42EB-44BE-A8D9-B2BE687F53AC}" name="Coluna1"/>
-    <tableColumn id="5" xr3:uid="{F95E8397-AFCE-4A1B-8DB6-D4D18DB74821}" name="Coluna2"/>
+    <tableColumn id="4" xr3:uid="{77371F62-42EB-44BE-A8D9-B2BE687F53AC}" name="Usado"/>
+    <tableColumn id="5" xr3:uid="{F95E8397-AFCE-4A1B-8DB6-D4D18DB74821}" name="Por Quem"/>
+    <tableColumn id="6" xr3:uid="{BDB3D452-35DD-4EC1-82A8-589786360658}" name="Estado"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1619,13 +1626,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F59"/>
+  <dimension ref="B1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,13 +1640,16 @@
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="3" max="3" width="29.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1649,14 +1659,17 @@
       <c r="D2" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="F2" s="26" t="s">
+      <c r="E2" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -1666,8 +1679,11 @@
       <c r="D3" s="25">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1677,8 +1693,11 @@
       <c r="D4" s="25">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1688,8 +1707,11 @@
       <c r="D5" s="25">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1700,7 +1722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -1711,7 +1733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -1722,7 +1744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1733,7 +1755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -1747,10 +1769,11 @@
         <v>185</v>
       </c>
       <c r="F10" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="I10" s="26"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -1761,7 +1784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -1772,7 +1795,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -1783,7 +1806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -1794,7 +1817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -1805,7 +1828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -1816,7 +1839,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>8</v>
       </c>
@@ -1827,7 +1850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>8</v>
       </c>
@@ -1838,7 +1861,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>8</v>
       </c>
@@ -1849,7 +1872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>8</v>
       </c>
@@ -1860,7 +1883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -1870,8 +1893,17 @@
       <c r="D21" s="25">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>185</v>
+      </c>
+      <c r="F21" t="s">
+        <v>186</v>
+      </c>
+      <c r="G21" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>18</v>
       </c>
@@ -1881,8 +1913,17 @@
       <c r="D22" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>185</v>
+      </c>
+      <c r="F22" t="s">
+        <v>193</v>
+      </c>
+      <c r="G22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>18</v>
       </c>
@@ -1893,7 +1934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>18</v>
       </c>
@@ -1904,7 +1945,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>18</v>
       </c>
@@ -1915,7 +1956,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>18</v>
       </c>
@@ -1926,7 +1967,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>18</v>
       </c>
@@ -1937,7 +1978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>26</v>
       </c>
@@ -1948,7 +1989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>26</v>
       </c>
@@ -1959,7 +2000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>26</v>
       </c>
@@ -1970,7 +2011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>26</v>
       </c>
@@ -1981,7 +2022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>26</v>
       </c>
@@ -2290,7 +2331,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>